<commit_message>
Ensure GA works with lib.c
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/icosahedron/icosahedron_AgAu_data.xlsx
+++ b/data/bimetallic_results/icosahedron/icosahedron_AgAu_data.xlsx
@@ -461,7 +461,7 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>-2.214498069149535</v>
+        <v>-2.283908985393195</v>
       </c>
       <c r="G3">
         <v>-0.01380053847560303</v>
@@ -484,7 +484,7 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <v>-2.276566903375702</v>
+        <v>-2.416088453551624</v>
       </c>
       <c r="G4">
         <v>-0.02760107695120695</v>
@@ -507,7 +507,7 @@
         <v>3</v>
       </c>
       <c r="F5">
-        <v>-2.338635737601868</v>
+        <v>-2.548967639398655</v>
       </c>
       <c r="G5">
         <v>-0.04140161542681042</v>
@@ -530,7 +530,7 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <v>-2.396338640727786</v>
+        <v>-2.681846825245684</v>
       </c>
       <c r="G6">
         <v>-0.0508362228021646</v>
@@ -553,7 +553,7 @@
         <v>5</v>
       </c>
       <c r="F7">
-        <v>-2.449675612753454</v>
+        <v>-2.814726011092715</v>
       </c>
       <c r="G7">
         <v>-0.0559048990772697</v>
@@ -576,7 +576,7 @@
         <v>6</v>
       </c>
       <c r="F8">
-        <v>-2.503012584779122</v>
+        <v>-2.948304914628344</v>
       </c>
       <c r="G8">
         <v>-0.06097357535237435</v>
@@ -599,7 +599,7 @@
         <v>7</v>
       </c>
       <c r="F9">
-        <v>-2.551983625704541</v>
+        <v>-3.081184100475374</v>
       </c>
       <c r="G9">
         <v>-0.06167632052723038</v>
@@ -622,7 +622,7 @@
         <v>8</v>
       </c>
       <c r="F10">
-        <v>-2.60095466662996</v>
+        <v>-3.214763004011005</v>
       </c>
       <c r="G10">
         <v>-0.06237906570208596</v>
@@ -645,7 +645,7 @@
         <v>9</v>
       </c>
       <c r="F11">
-        <v>-2.64555977645513</v>
+        <v>-3.348341907546635</v>
       </c>
       <c r="G11">
         <v>-0.05871587977669313</v>
@@ -668,7 +668,7 @@
         <v>10</v>
       </c>
       <c r="F12">
-        <v>-2.68579895518005</v>
+        <v>-3.481920811082266</v>
       </c>
       <c r="G12">
         <v>-0.05068676275105033</v>
@@ -691,7 +691,7 @@
         <v>11</v>
       </c>
       <c r="F13">
-        <v>-2.726038133904971</v>
+        <v>-3.616199432306497</v>
       </c>
       <c r="G13">
         <v>-0.04265764572540776</v>
@@ -714,7 +714,7 @@
         <v>12</v>
       </c>
       <c r="F14">
-        <v>-2.766277312629891</v>
+        <v>-3.75117777121933</v>
       </c>
       <c r="G14">
         <v>-0.03462852869976407</v>
@@ -737,7 +737,7 @@
         <v>13</v>
       </c>
       <c r="F15">
-        <v>-2.779917079680689</v>
+        <v>-3.855339157786533</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -783,7 +783,7 @@
         <v>1</v>
       </c>
       <c r="F17">
-        <v>-2.486224135747408</v>
+        <v>-2.497660976620755</v>
       </c>
       <c r="G17">
         <v>-0.006942494621560158</v>
@@ -806,7 +806,7 @@
         <v>2</v>
       </c>
       <c r="F18">
-        <v>-2.503584231624124</v>
+        <v>-2.529112362948664</v>
       </c>
       <c r="G18">
         <v>-0.01123053966529142</v>
@@ -829,7 +829,7 @@
         <v>3</v>
       </c>
       <c r="F19">
-        <v>-2.52094432750084</v>
+        <v>-2.560563749276572</v>
       </c>
       <c r="G19">
         <v>-0.01551858470902134</v>
@@ -852,7 +852,7 @@
         <v>4</v>
       </c>
       <c r="F20">
-        <v>-2.538304423377556</v>
+        <v>-2.59201513560448</v>
       </c>
       <c r="G20">
         <v>-0.0198066297527526</v>
@@ -875,7 +875,7 @@
         <v>5</v>
       </c>
       <c r="F21">
-        <v>-2.554934822284575</v>
+        <v>-2.623466521932388</v>
       </c>
       <c r="G21">
         <v>-0.02336497782678615</v>
@@ -898,7 +898,7 @@
         <v>6</v>
       </c>
       <c r="F22">
-        <v>-2.571364927565576</v>
+        <v>-2.654917908260296</v>
       </c>
       <c r="G22">
         <v>-0.02672303227480155</v>
@@ -921,7 +921,7 @@
         <v>7</v>
       </c>
       <c r="F23">
-        <v>-2.587795032846577</v>
+        <v>-2.686369294588204</v>
       </c>
       <c r="G23">
         <v>-0.0295074114918692</v>
@@ -944,7 +944,7 @@
         <v>8</v>
       </c>
       <c r="F24">
-        <v>-2.604225138127578</v>
+        <v>-2.717820680916112</v>
       </c>
       <c r="G24">
         <v>-0.03343914117083324</v>
@@ -967,7 +967,7 @@
         <v>9</v>
       </c>
       <c r="F25">
-        <v>-2.62045494978256</v>
+        <v>-2.74927206724402</v>
       </c>
       <c r="G25">
         <v>-0.03659690199282917</v>
@@ -990,7 +990,7 @@
         <v>10</v>
       </c>
       <c r="F26">
-        <v>-2.63688505506356</v>
+        <v>-2.780723453571928</v>
       </c>
       <c r="G26">
         <v>-0.03889614975348765</v>
@@ -1013,7 +1013,7 @@
         <v>11</v>
       </c>
       <c r="F27">
-        <v>-2.652703759175079</v>
+        <v>-2.812174839899834</v>
       </c>
       <c r="G27">
         <v>-0.04270160971937775</v>
@@ -1036,7 +1036,7 @@
         <v>12</v>
       </c>
       <c r="F28">
-        <v>-2.668322169660577</v>
+        <v>-2.843626226227742</v>
       </c>
       <c r="G28">
         <v>-0.04524796937189035</v>
@@ -1059,7 +1059,7 @@
         <v>13</v>
       </c>
       <c r="F29">
-        <v>-2.683887215931507</v>
+        <v>-2.873173192687904</v>
       </c>
       <c r="G29">
         <v>-0.04605264363318895</v>
@@ -1082,7 +1082,7 @@
         <v>14</v>
       </c>
       <c r="F30">
-        <v>-2.698665298010269</v>
+        <v>-2.902720159148066</v>
       </c>
       <c r="G30">
         <v>-0.04818789574223636</v>
@@ -1105,7 +1105,7 @@
         <v>15</v>
       </c>
       <c r="F31">
-        <v>-2.713918300803698</v>
+        <v>-2.932267125608218</v>
       </c>
       <c r="G31">
         <v>-0.05115025948633112</v>
@@ -1128,7 +1128,7 @@
         <v>16</v>
       </c>
       <c r="F32">
-        <v>-2.72934621075941</v>
+        <v>-2.961814092068379</v>
       </c>
       <c r="G32">
         <v>-0.05324123970811123</v>
@@ -1151,7 +1151,7 @@
         <v>17</v>
       </c>
       <c r="F33">
-        <v>-2.745443428189076</v>
+        <v>-2.991361058528541</v>
       </c>
       <c r="G33">
         <v>-0.05370316983454138</v>
@@ -1174,7 +1174,7 @@
         <v>18</v>
       </c>
       <c r="F34">
-        <v>-2.759051433061438</v>
+        <v>-3.020908024988696</v>
       </c>
       <c r="G34">
         <v>-0.05712402713514519</v>
@@ -1197,7 +1197,7 @@
         <v>19</v>
       </c>
       <c r="F35">
-        <v>-2.774053545829339</v>
+        <v>-3.050454991448855</v>
       </c>
       <c r="G35">
         <v>-0.05708417721051928</v>
@@ -1220,7 +1220,7 @@
         <v>20</v>
       </c>
       <c r="F36">
-        <v>-2.787897441533201</v>
+        <v>-3.080001957909011</v>
       </c>
       <c r="G36">
         <v>-0.05854144716382148</v>
@@ -1243,7 +1243,7 @@
         <v>21</v>
       </c>
       <c r="F37">
-        <v>-2.801318787196749</v>
+        <v>-3.109056859205772</v>
       </c>
       <c r="G37">
         <v>-0.06032639887065772</v>
@@ -1266,7 +1266,7 @@
         <v>22</v>
       </c>
       <c r="F38">
-        <v>-2.816220061623838</v>
+        <v>-3.13761969533912</v>
       </c>
       <c r="G38">
         <v>-0.06034092347921649</v>
@@ -1289,7 +1289,7 @@
         <v>23</v>
       </c>
       <c r="F39">
-        <v>-2.829472515087664</v>
+        <v>-3.167166661799279</v>
       </c>
       <c r="G39">
         <v>-0.06168443972221138</v>
@@ -1312,7 +1312,7 @@
         <v>24</v>
       </c>
       <c r="F40">
-        <v>-2.843685596617266</v>
+        <v>-3.196221563096033</v>
       </c>
       <c r="G40">
         <v>-0.06374678633275654</v>
@@ -1335,7 +1335,7 @@
         <v>25</v>
       </c>
       <c r="F41">
-        <v>-2.857064319794164</v>
+        <v>-3.224292334065978</v>
       </c>
       <c r="G41">
         <v>-0.06402098374445675</v>
@@ -1358,7 +1358,7 @@
         <v>26</v>
       </c>
       <c r="F42">
-        <v>-2.870679225073467</v>
+        <v>-3.253347235362731</v>
       </c>
       <c r="G42">
         <v>-0.06217899574556873</v>
@@ -1381,7 +1381,7 @@
         <v>27</v>
       </c>
       <c r="F43">
-        <v>-2.882917498195412</v>
+        <v>-3.281910071496083</v>
       </c>
       <c r="G43">
         <v>-0.06258543292437579</v>
@@ -1404,7 +1404,7 @@
         <v>28</v>
       </c>
       <c r="F44">
-        <v>-2.896552007945953</v>
+        <v>-3.310472907629436</v>
       </c>
       <c r="G44">
         <v>-0.06425774933534556</v>
@@ -1427,7 +1427,7 @@
         <v>29</v>
       </c>
       <c r="F45">
-        <v>-2.909037083410069</v>
+        <v>-3.339035743762789</v>
       </c>
       <c r="G45">
         <v>-0.06373801896063247</v>
@@ -1450,7 +1450,7 @@
         <v>30</v>
       </c>
       <c r="F46">
-        <v>-2.922663740735903</v>
+        <v>-3.367106514732737</v>
       </c>
       <c r="G46">
         <v>-0.06396081110806562</v>
@@ -1473,7 +1473,7 @@
         <v>31</v>
       </c>
       <c r="F47">
-        <v>-2.934903896228521</v>
+        <v>-3.395669350866083</v>
       </c>
       <c r="G47">
         <v>-0.06261238288499471</v>
@@ -1496,7 +1496,7 @@
         <v>32</v>
       </c>
       <c r="F48">
-        <v>-2.947074879447785</v>
+        <v>-3.424232186999435</v>
       </c>
       <c r="G48">
         <v>-0.06212700981316766</v>
@@ -1519,7 +1519,7 @@
         <v>33</v>
       </c>
       <c r="F49">
-        <v>-2.960137717826206</v>
+        <v>-3.452302957969381</v>
       </c>
       <c r="G49">
         <v>-0.06096447684267692</v>
@@ -1542,7 +1542,7 @@
         <v>34</v>
       </c>
       <c r="F50">
-        <v>-2.972841927431347</v>
+        <v>-3.479389598612523</v>
       </c>
       <c r="G50">
         <v>-0.06060762370513217</v>
@@ -1565,7 +1565,7 @@
         <v>35</v>
       </c>
       <c r="F51">
-        <v>-2.984137029946916</v>
+        <v>-3.50746036958247</v>
       </c>
       <c r="G51">
         <v>-0.06040566049956797</v>
@@ -1588,7 +1588,7 @@
         <v>36</v>
       </c>
       <c r="F52">
-        <v>-2.996003116458004</v>
+        <v>-3.535039075389013</v>
       </c>
       <c r="G52">
         <v>-0.05760801756264844</v>
@@ -1611,7 +1611,7 @@
         <v>37</v>
       </c>
       <c r="F53">
-        <v>-3.007959862084359</v>
+        <v>-3.562617781195557</v>
       </c>
       <c r="G53">
         <v>-0.05714041149990923</v>
@@ -1634,7 +1634,7 @@
         <v>38</v>
       </c>
       <c r="F54">
-        <v>-3.018190497408225</v>
+        <v>-3.590196487002101</v>
       </c>
       <c r="G54">
         <v>-0.05524297546192114</v>
@@ -1657,7 +1657,7 @@
         <v>39</v>
       </c>
       <c r="F55">
-        <v>-3.029900176051246</v>
+        <v>-3.617775192808644</v>
       </c>
       <c r="G55">
         <v>-0.05321325474830263</v>
@@ -1680,7 +1680,7 @@
         <v>40</v>
       </c>
       <c r="F56">
-        <v>-3.040358228978684</v>
+        <v>-3.645353898615188</v>
       </c>
       <c r="G56">
         <v>-0.05103918776283811</v>
@@ -1703,7 +1703,7 @@
         <v>41</v>
       </c>
       <c r="F57">
-        <v>-3.052384101969868</v>
+        <v>-3.672932604421731</v>
       </c>
       <c r="G57">
         <v>-0.05001794197823095</v>
@@ -1726,7 +1726,7 @@
         <v>42</v>
       </c>
       <c r="F58">
-        <v>-3.062267905475509</v>
+        <v>-3.700511310228275</v>
       </c>
       <c r="G58">
         <v>-0.04563620820983105</v>
@@ -1749,7 +1749,7 @@
         <v>43</v>
       </c>
       <c r="F59">
-        <v>-3.073311309100795</v>
+        <v>-3.726649399536589</v>
       </c>
       <c r="G59">
         <v>-0.04369633774672432</v>
@@ -1772,7 +1772,7 @@
         <v>44</v>
       </c>
       <c r="F60">
-        <v>-3.084209292948315</v>
+        <v>-3.756203857030933</v>
       </c>
       <c r="G60">
         <v>-0.04282946600409965</v>
@@ -1795,7 +1795,7 @@
         <v>45</v>
       </c>
       <c r="F61">
-        <v>-3.093711304808402</v>
+        <v>-3.78170163320847</v>
       </c>
       <c r="G61">
         <v>-0.03825202560810936</v>
@@ -1818,7 +1818,7 @@
         <v>46</v>
       </c>
       <c r="F62">
-        <v>-3.1030176100409</v>
+        <v>-3.806559096255227</v>
       </c>
       <c r="G62">
         <v>-0.03495969108860658</v>
@@ -1841,7 +1841,7 @@
         <v>47</v>
       </c>
       <c r="F63">
-        <v>-3.112323915273397</v>
+        <v>-3.831416559301985</v>
       </c>
       <c r="G63">
         <v>-0.03172793583022576</v>
@@ -1864,7 +1864,7 @@
         <v>48</v>
       </c>
       <c r="F64">
-        <v>-3.121630220505895</v>
+        <v>-3.856274022348742</v>
       </c>
       <c r="G64">
         <v>-0.02796219022973762</v>
@@ -1887,7 +1887,7 @@
         <v>49</v>
       </c>
       <c r="F65">
-        <v>-3.130936525738392</v>
+        <v>-3.880491172264722</v>
       </c>
       <c r="G65">
         <v>-0.02419644462924991</v>
@@ -1910,7 +1910,7 @@
         <v>50</v>
       </c>
       <c r="F66">
-        <v>-3.14024283097089</v>
+        <v>-3.904068009049922</v>
       </c>
       <c r="G66">
         <v>-0.02043069902876224</v>
@@ -1933,7 +1933,7 @@
         <v>51</v>
       </c>
       <c r="F67">
-        <v>-3.149549136203386</v>
+        <v>-3.927644845835124</v>
       </c>
       <c r="G67">
         <v>-0.01666495342827365</v>
@@ -1956,7 +1956,7 @@
         <v>52</v>
       </c>
       <c r="F68">
-        <v>-3.158855441435884</v>
+        <v>-3.950581369489547</v>
       </c>
       <c r="G68">
         <v>-0.0128992078277855</v>
@@ -1979,7 +1979,7 @@
         <v>53</v>
       </c>
       <c r="F69">
-        <v>-3.167627756326274</v>
+        <v>-3.972877580013191</v>
       </c>
       <c r="G69">
         <v>-0.008599471885190044</v>
@@ -2002,7 +2002,7 @@
         <v>54</v>
       </c>
       <c r="F70">
-        <v>-3.176400071216664</v>
+        <v>-3.995173790536836</v>
       </c>
       <c r="G70">
         <v>-0.004299735942595022</v>
@@ -2025,7 +2025,7 @@
         <v>55</v>
       </c>
       <c r="F71">
-        <v>-3.185172386107054</v>
+        <v>-4.017470001060481</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -7499,7 +7499,7 @@
         <v>652</v>
       </c>
       <c r="F309">
-        <v>-2.961143168579724</v>
+        <v>-3.018311655611262</v>
       </c>
       <c r="G309">
         <v>-0.02337841381927053</v>
@@ -7522,7 +7522,7 @@
         <v>1305</v>
       </c>
       <c r="F310">
-        <v>-3.061877308999199</v>
+        <v>-3.17845730755005</v>
       </c>
       <c r="G310">
         <v>-0.04104585189671672</v>
@@ -7545,7 +7545,7 @@
         <v>1957</v>
       </c>
       <c r="F311">
-        <v>-3.156838700681143</v>
+        <v>-3.334234127884221</v>
       </c>
       <c r="G311">
         <v>-0.05269650776244039</v>
@@ -7568,7 +7568,7 @@
         <v>2610</v>
       </c>
       <c r="F312">
-        <v>-3.245695609522403</v>
+        <v>-3.486326736666184</v>
       </c>
       <c r="G312">
         <v>-0.05842104686373228</v>
@@ -7591,7 +7591,7 @@
         <v>3262</v>
       </c>
       <c r="F313">
-        <v>-3.330630497995005</v>
+        <v>-3.634333330164532</v>
       </c>
       <c r="G313">
         <v>-0.06011988500389776</v>
@@ -7614,7 +7614,7 @@
         <v>3915</v>
       </c>
       <c r="F314">
-        <v>-3.411442136844541</v>
+        <v>-3.780268381506738</v>
       </c>
       <c r="G314">
         <v>-0.05775801438557937</v>
@@ -7637,7 +7637,7 @@
         <v>4567</v>
       </c>
       <c r="F315">
-        <v>-3.487362754576969</v>
+        <v>-3.922024566550103</v>
       </c>
       <c r="G315">
         <v>-0.05048898625023235</v>
@@ -7660,7 +7660,7 @@
         <v>5220</v>
       </c>
       <c r="F316">
-        <v>-3.558888491972898</v>
+        <v>-4.057763571624702</v>
       </c>
       <c r="G316">
         <v>-0.03877803683569647</v>
@@ -7683,7 +7683,7 @@
         <v>5872</v>
       </c>
       <c r="F317">
-        <v>-3.625129809752895</v>
+        <v>-4.188725883400633</v>
       </c>
       <c r="G317">
         <v>-0.02186995315499513</v>
@@ -7706,7 +7706,7 @@
         <v>6525</v>
       </c>
       <c r="F318">
-        <v>-3.686536787815441</v>
+        <v>-4.314433232740556</v>
       </c>
       <c r="G318">
         <v>0</v>

</xml_diff>

<commit_message>
started adding doc strings and organizing ga.py
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/icosahedron/icosahedron_AgAu_data.xlsx
+++ b/data/bimetallic_results/icosahedron/icosahedron_AgAu_data.xlsx
@@ -1013,7 +1013,7 @@
         <v>11</v>
       </c>
       <c r="F27">
-        <v>-2.652703759175079</v>
+        <v>-2.652986050626902</v>
       </c>
       <c r="G27">
         <v>-0.04270160971937775</v>
@@ -1036,7 +1036,7 @@
         <v>12</v>
       </c>
       <c r="F28">
-        <v>-2.668322169660577</v>
+        <v>-2.6686044611124</v>
       </c>
       <c r="G28">
         <v>-0.04524796937189035</v>
@@ -1082,7 +1082,7 @@
         <v>14</v>
       </c>
       <c r="F30">
-        <v>-2.698665298010269</v>
+        <v>-2.699072209774548</v>
       </c>
       <c r="G30">
         <v>-0.04818789574223636</v>
@@ -1105,7 +1105,7 @@
         <v>15</v>
       </c>
       <c r="F31">
-        <v>-2.713918300803698</v>
+        <v>-2.714859512459772</v>
       </c>
       <c r="G31">
         <v>-0.05115025948633112</v>
@@ -1243,7 +1243,7 @@
         <v>21</v>
       </c>
       <c r="F37">
-        <v>-2.801318787196749</v>
+        <v>-2.80157734158545</v>
       </c>
       <c r="G37">
         <v>-0.06032639887065772</v>
@@ -1266,7 +1266,7 @@
         <v>22</v>
       </c>
       <c r="F38">
-        <v>-2.816220061623838</v>
+        <v>-2.816566583892378</v>
       </c>
       <c r="G38">
         <v>-0.06034092347921649</v>
@@ -1289,7 +1289,7 @@
         <v>23</v>
       </c>
       <c r="F39">
-        <v>-2.829472515087664</v>
+        <v>-2.829590046931646</v>
       </c>
       <c r="G39">
         <v>-0.06168443972221138</v>
@@ -1381,7 +1381,7 @@
         <v>27</v>
       </c>
       <c r="F43">
-        <v>-2.882917498195412</v>
+        <v>-2.883086390395136</v>
       </c>
       <c r="G43">
         <v>-0.06258543292437579</v>
@@ -1634,7 +1634,7 @@
         <v>38</v>
       </c>
       <c r="F54">
-        <v>-3.018190497408225</v>
+        <v>-3.018738431717223</v>
       </c>
       <c r="G54">
         <v>-0.05524297546192114</v>
@@ -1680,7 +1680,7 @@
         <v>40</v>
       </c>
       <c r="F56">
-        <v>-3.040358228978684</v>
+        <v>-3.041138212798205</v>
       </c>
       <c r="G56">
         <v>-0.05103918776283811</v>
@@ -1726,7 +1726,7 @@
         <v>42</v>
       </c>
       <c r="F58">
-        <v>-3.062267905475509</v>
+        <v>-3.062349903301314</v>
       </c>
       <c r="G58">
         <v>-0.04563620820983105</v>

</xml_diff>

<commit_message>
changed __main__ to run all 12 combinations
</commit_message>
<xml_diff>
--- a/data/bimetallic_results/icosahedron/icosahedron_AgAu_data.xlsx
+++ b/data/bimetallic_results/icosahedron/icosahedron_AgAu_data.xlsx
@@ -1657,7 +1657,7 @@
         <v>39</v>
       </c>
       <c r="F55">
-        <v>-3.029900176051246</v>
+        <v>-3.030887928094577</v>
       </c>
       <c r="G55">
         <v>-0.05321325474830263</v>
@@ -2140,7 +2140,7 @@
         <v>4</v>
       </c>
       <c r="F76">
-        <v>-2.634339705556114</v>
+        <v>-2.634422043320821</v>
       </c>
       <c r="G76">
         <v>-0.00893584863858754</v>
@@ -2393,7 +2393,7 @@
         <v>15</v>
       </c>
       <c r="F87">
-        <v>-2.710337023541463</v>
+        <v>-2.710974831310411</v>
       </c>
       <c r="G87">
         <v>-0.02811118376813981</v>
@@ -2508,7 +2508,7 @@
         <v>20</v>
       </c>
       <c r="F92">
-        <v>-2.742350759502981</v>
+        <v>-2.74237999266129</v>
       </c>
       <c r="G92">
         <v>-0.03422312651608106</v>
@@ -2669,7 +2669,7 @@
         <v>27</v>
       </c>
       <c r="F99">
-        <v>-2.786308839529481</v>
+        <v>-2.786424091150784</v>
       </c>
       <c r="G99">
         <v>-0.0409597003159865</v>
@@ -2761,7 +2761,7 @@
         <v>31</v>
       </c>
       <c r="F103">
-        <v>-2.810768084772148</v>
+        <v>-2.810912887110952</v>
       </c>
       <c r="G103">
         <v>-0.04563919710637787</v>
@@ -3313,7 +3313,7 @@
         <v>55</v>
       </c>
       <c r="F127">
-        <v>-2.951799739679519</v>
+        <v>-2.952406707047291</v>
       </c>
       <c r="G127">
         <v>-0.06294850770330052</v>
@@ -3382,7 +3382,7 @@
         <v>58</v>
       </c>
       <c r="F130">
-        <v>-2.968461319777281</v>
+        <v>-2.968649756275445</v>
       </c>
       <c r="G130">
         <v>-0.06312515460966228</v>
@@ -3589,7 +3589,7 @@
         <v>67</v>
       </c>
       <c r="F139">
-        <v>-3.016300422119442</v>
+        <v>-3.016451958581431</v>
       </c>
       <c r="G139">
         <v>-0.06394639529128265</v>
@@ -3957,7 +3957,7 @@
         <v>83</v>
       </c>
       <c r="F155">
-        <v>-3.098388768444609</v>
+        <v>-3.098720162452815</v>
       </c>
       <c r="G155">
         <v>-0.06435983074914242</v>
@@ -3980,7 +3980,7 @@
         <v>84</v>
       </c>
       <c r="F156">
-        <v>-3.103587831010045</v>
+        <v>-3.103888996016249</v>
       </c>
       <c r="G156">
         <v>-0.06433114772274973</v>
@@ -4716,7 +4716,7 @@
         <v>116</v>
       </c>
       <c r="F188">
-        <v>-3.248074837837004</v>
+        <v>-3.248573686202946</v>
       </c>
       <c r="G188">
         <v>-0.04379921470243286</v>
@@ -4831,7 +4831,7 @@
         <v>121</v>
       </c>
       <c r="F193">
-        <v>-3.268780813995622</v>
+        <v>-3.268854256156096</v>
       </c>
       <c r="G193">
         <v>-0.0378437283319274</v>
@@ -4969,7 +4969,7 @@
         <v>127</v>
       </c>
       <c r="F199">
-        <v>-3.292452338402729</v>
+        <v>-3.293266493437927</v>
       </c>
       <c r="G199">
         <v>-0.03113329506051993</v>
@@ -5107,7 +5107,7 @@
         <v>133</v>
       </c>
       <c r="F205">
-        <v>-3.315468475507523</v>
+        <v>-3.315785837784002</v>
       </c>
       <c r="G205">
         <v>-0.02290637012843255</v>
@@ -5659,7 +5659,7 @@
         <v>278</v>
       </c>
       <c r="F229">
-        <v>-3.409415563922665</v>
+        <v>-3.409472200087178</v>
       </c>
       <c r="G229">
         <v>-0.02387749183716054</v>
@@ -5774,7 +5774,7 @@
         <v>168</v>
       </c>
       <c r="F234">
-        <v>-3.024736934229871</v>
+        <v>-3.025044083377698</v>
       </c>
       <c r="G234">
         <v>-0.05457474792285844</v>
@@ -6096,7 +6096,7 @@
         <v>553</v>
       </c>
       <c r="F248">
-        <v>-3.308552076666951</v>
+        <v>-3.308644466035405</v>
       </c>
       <c r="G248">
         <v>-0.06043021574715146</v>
@@ -6740,7 +6740,7 @@
         <v>286</v>
       </c>
       <c r="F276">
-        <v>-2.930265239370734</v>
+        <v>-2.930434023534275</v>
       </c>
       <c r="G276">
         <v>-0.02416348175684568</v>
@@ -6786,7 +6786,7 @@
         <v>860</v>
       </c>
       <c r="F278">
-        <v>-3.124235535679953</v>
+        <v>-3.124291398270081</v>
       </c>
       <c r="G278">
         <v>-0.05329181316478926</v>
@@ -7177,7 +7177,7 @@
         <v>3483</v>
       </c>
       <c r="F295">
-        <v>-3.60195741117442</v>
+        <v>-3.60204674254797</v>
       </c>
       <c r="G295">
         <v>-0.02199392333322014</v>
@@ -7545,7 +7545,7 @@
         <v>1957</v>
       </c>
       <c r="F311">
-        <v>-3.156838700681143</v>
+        <v>-3.156904829166496</v>
       </c>
       <c r="G311">
         <v>-0.05269650776244039</v>
@@ -7568,7 +7568,7 @@
         <v>2610</v>
       </c>
       <c r="F312">
-        <v>-3.245695609522403</v>
+        <v>-3.245721287485625</v>
       </c>
       <c r="G312">
         <v>-0.05842104686373228</v>

</xml_diff>